<commit_message>
Test - Konacno - JavaScript
</commit_message>
<xml_diff>
--- a/JavaScript/10. Cas - Test/Test-JavaScript-1.deo.xlsx
+++ b/JavaScript/10. Cas - Test/Test-JavaScript-1.deo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dženan Košuta\GitHub\IT Camp - 1. grupa\JavaScript\10. Cas - Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3E3F5D-3186-42DB-A0A1-526B0C84ADBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1305FD25-39E7-4283-A3C9-ED5EA679D74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>TEST</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Mervan Bronja</t>
+  </si>
+  <si>
+    <t>Popravni</t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +550,7 @@
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -558,7 +561,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -577,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="14"/>
@@ -592,7 +595,7 @@
       </c>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -616,7 +619,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -640,7 +643,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -664,7 +667,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -688,7 +691,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -712,7 +715,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -735,8 +738,11 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -760,7 +766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -784,7 +790,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -808,7 +814,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -832,39 +838,55 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="2">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3">
+        <v>20</v>
+      </c>
+      <c r="E14" s="5">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3">
+        <v>20</v>
+      </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="2">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3">
+        <v>20</v>
+      </c>
+      <c r="E15" s="5">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3">
+        <v>5</v>
+      </c>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>

</xml_diff>